<commit_message>
refactor: Remove unnecessary code in Vino.py, InterfazExcel.py, GestorRankingVinos.py, Bodega.py, and Varietal.py
</commit_message>
<xml_diff>
--- a/RankingVinos.xlsx
+++ b/RankingVinos.xlsx
@@ -11,6 +11,101 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+  <si>
+    <t>Cabernet Franc</t>
+  </si>
+  <si>
+    <t>Bodega Cinco</t>
+  </si>
+  <si>
+    <t>Famoso por sus vinos tintos de alta calidad</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Cabernet FrancSauvignon Blanc es una variedad de uva blanca conocida por su frescura y sus aromas herbáceos y cítricos.Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Sangiovese es una variedad de uva tinta que se asocia principalmente con los vinos italianos, conocidos por su acidez y sabor a frutas rojas.</t>
+  </si>
+  <si>
+    <t>Malbec</t>
+  </si>
+  <si>
+    <t>MalbecMalbec</t>
+  </si>
+  <si>
+    <t>Torrontés Clásico</t>
+  </si>
+  <si>
+    <t>Bodega Dos</t>
+  </si>
+  <si>
+    <t>Reconocida por sus Malbecs</t>
+  </si>
+  <si>
+    <t>Torrontés ClásicoMourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
+  </si>
+  <si>
+    <t>Merlot Reserva</t>
+  </si>
+  <si>
+    <t>Bodega Tres</t>
+  </si>
+  <si>
+    <t>Región importante de San Juan</t>
+  </si>
+  <si>
+    <t>Merlot ReservaMerlot Reserva</t>
+  </si>
+  <si>
+    <t>Riesling</t>
+  </si>
+  <si>
+    <t>Bodega Ocho</t>
+  </si>
+  <si>
+    <t>RieslingRiesling</t>
+  </si>
+  <si>
+    <t>Chardonnay</t>
+  </si>
+  <si>
+    <t>Bodega Cuatro</t>
+  </si>
+  <si>
+    <t>Sémillon es una variedad de uva blanca que se utiliza en la producción de vinos blancos secos, dulces y también vinos de postre.Pinot Grigio es una variedad de uva blanca que produce vinos blancos ligeros y refrescantes, con notas cítricas y florales.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
+  </si>
+  <si>
+    <t>Zinfandel</t>
+  </si>
+  <si>
+    <t>ZinfandelZinfandel</t>
+  </si>
+  <si>
+    <t>Cabernet</t>
+  </si>
+  <si>
+    <t>Bodega Seis</t>
+  </si>
+  <si>
+    <t>CabernetMerlot es una variedad de uva tinta que se caracteriza por su suavidad y sabor frutal en los vinos.Pinot Noir es una variedad de uva tinta que se asocia con vinos ligeros, elegantes y afrutados.</t>
+  </si>
+  <si>
+    <t>Pinot Noir</t>
+  </si>
+  <si>
+    <t>Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.Tannat es una variedad de uva tinta que se asocia principalmente con los vinos de Uruguay, conocidos por su estructura tánica y sabor intenso.</t>
+  </si>
+  <si>
+    <t>Torrontés</t>
+  </si>
+  <si>
+    <t>TorrontésRiesling es una variedad de uva blanca que puede producir desde vinos secos y refrescantes hasta vinos dulces y aromáticos.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,12 +435,243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1300</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1200</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>9.199999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1250</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>1350</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>1350</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>1100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>8.324999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>1300</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>8.300000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>1500</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>1150</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10">
+        <v>8.199999999999999</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: Remove unnecessary code in main1.py, Vino.py, InterfazExcel.py, GestorRankingVinos.py, Bodega.py, and Varietal.py
</commit_message>
<xml_diff>
--- a/RankingVinos.xlsx
+++ b/RankingVinos.xlsx
@@ -14,96 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
-  <si>
-    <t>Cabernet Franc</t>
-  </si>
-  <si>
-    <t>Bodega Cinco</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+  <si>
+    <t>Torrontés Clásico</t>
+  </si>
+  <si>
+    <t>Bodega Dos</t>
+  </si>
+  <si>
+    <t>Reconocida por sus Malbecs</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Torrontés ClásicoMourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
+  </si>
+  <si>
+    <t>Cabernet Sauvignon</t>
+  </si>
+  <si>
+    <t>Bodega Uno</t>
   </si>
   <si>
     <t>Famoso por sus vinos tintos de alta calidad</t>
   </si>
   <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Cabernet FrancSauvignon Blanc es una variedad de uva blanca conocida por su frescura y sus aromas herbáceos y cítricos.Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Sangiovese es una variedad de uva tinta que se asocia principalmente con los vinos italianos, conocidos por su acidez y sabor a frutas rojas.</t>
-  </si>
-  <si>
-    <t>Malbec</t>
-  </si>
-  <si>
-    <t>MalbecMalbec</t>
-  </si>
-  <si>
-    <t>Torrontés Clásico</t>
-  </si>
-  <si>
-    <t>Bodega Dos</t>
-  </si>
-  <si>
-    <t>Reconocida por sus Malbecs</t>
-  </si>
-  <si>
-    <t>Torrontés ClásicoMourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
-  </si>
-  <si>
-    <t>Merlot Reserva</t>
-  </si>
-  <si>
-    <t>Bodega Tres</t>
-  </si>
-  <si>
-    <t>Región importante de San Juan</t>
-  </si>
-  <si>
-    <t>Merlot ReservaMerlot Reserva</t>
-  </si>
-  <si>
-    <t>Riesling</t>
-  </si>
-  <si>
-    <t>Bodega Ocho</t>
-  </si>
-  <si>
-    <t>RieslingRiesling</t>
-  </si>
-  <si>
-    <t>Chardonnay</t>
-  </si>
-  <si>
-    <t>Bodega Cuatro</t>
-  </si>
-  <si>
-    <t>Sémillon es una variedad de uva blanca que se utiliza en la producción de vinos blancos secos, dulces y también vinos de postre.Pinot Grigio es una variedad de uva blanca que produce vinos blancos ligeros y refrescantes, con notas cítricas y florales.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
-  </si>
-  <si>
-    <t>Zinfandel</t>
-  </si>
-  <si>
-    <t>ZinfandelZinfandel</t>
-  </si>
-  <si>
-    <t>Cabernet</t>
-  </si>
-  <si>
-    <t>Bodega Seis</t>
-  </si>
-  <si>
-    <t>CabernetMerlot es una variedad de uva tinta que se caracteriza por su suavidad y sabor frutal en los vinos.Pinot Noir es una variedad de uva tinta que se asocia con vinos ligeros, elegantes y afrutados.</t>
-  </si>
-  <si>
-    <t>Pinot Noir</t>
-  </si>
-  <si>
-    <t>Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.Tannat es una variedad de uva tinta que se asocia principalmente con los vinos de Uruguay, conocidos por su estructura tánica y sabor intenso.</t>
-  </si>
-  <si>
-    <t>Torrontés</t>
-  </si>
-  <si>
-    <t>TorrontésRiesling es una variedad de uva blanca que puede producir desde vinos secos y refrescantes hasta vinos dulces y aromáticos.</t>
+    <t>Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.</t>
+  </si>
+  <si>
+    <t>Malbec Reserva</t>
+  </si>
+  <si>
+    <t>Mourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Grenache es una variedad de uva tinta que se utiliza en muchos vinos tintos y rosados, conocidos por su cuerpo y sabor afrutado.</t>
   </si>
 </sst>
 </file>
@@ -435,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -446,7 +389,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1300</v>
+        <v>1150</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -461,7 +404,7 @@
         <v>4</v>
       </c>
       <c r="G1">
-        <v>9.9</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -469,36 +412,36 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G2">
-        <v>9.199999999999999</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>1200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3">
-        <v>1150</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -507,168 +450,7 @@
         <v>10</v>
       </c>
       <c r="G3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>1250</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>1350</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>1350</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>1100</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7">
-        <v>8.324999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
-        <v>1300</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8">
-        <v>8.300000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9">
-        <v>1500</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9">
-        <v>8.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10">
-        <v>1150</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10">
-        <v>8.199999999999999</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Remove unnecessary code in GestorRankingVinos.py
</commit_message>
<xml_diff>
--- a/RankingVinos.xlsx
+++ b/RankingVinos.xlsx
@@ -14,7 +14,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+  <si>
+    <t>Cabernet Franc</t>
+  </si>
+  <si>
+    <t>Bodega Cinco</t>
+  </si>
+  <si>
+    <t>Famoso por sus vinos tintos de alta calidad</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Cabernet FrancSauvignon Blanc es una variedad de uva blanca conocida por su frescura y sus aromas herbáceos y cítricos.Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Sangiovese es una variedad de uva tinta que se asocia principalmente con los vinos italianos, conocidos por su acidez y sabor a frutas rojas.</t>
+  </si>
+  <si>
+    <t>Malbec</t>
+  </si>
+  <si>
+    <t>MalbecMalbec</t>
+  </si>
   <si>
     <t>Torrontés Clásico</t>
   </si>
@@ -25,28 +46,64 @@
     <t>Reconocida por sus Malbecs</t>
   </si>
   <si>
-    <t>Argentina</t>
-  </si>
-  <si>
     <t>Torrontés ClásicoMourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
   </si>
   <si>
-    <t>Cabernet Sauvignon</t>
-  </si>
-  <si>
-    <t>Bodega Uno</t>
-  </si>
-  <si>
-    <t>Famoso por sus vinos tintos de alta calidad</t>
-  </si>
-  <si>
-    <t>Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.</t>
-  </si>
-  <si>
-    <t>Malbec Reserva</t>
-  </si>
-  <si>
-    <t>Mourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Grenache es una variedad de uva tinta que se utiliza en muchos vinos tintos y rosados, conocidos por su cuerpo y sabor afrutado.</t>
+    <t>Merlot Reserva</t>
+  </si>
+  <si>
+    <t>Bodega Tres</t>
+  </si>
+  <si>
+    <t>Región importante de San Juan</t>
+  </si>
+  <si>
+    <t>Merlot ReservaMerlot Reserva</t>
+  </si>
+  <si>
+    <t>Riesling</t>
+  </si>
+  <si>
+    <t>Bodega Ocho</t>
+  </si>
+  <si>
+    <t>RieslingRiesling</t>
+  </si>
+  <si>
+    <t>Chardonnay</t>
+  </si>
+  <si>
+    <t>Bodega Cuatro</t>
+  </si>
+  <si>
+    <t>Sémillon es una variedad de uva blanca que se utiliza en la producción de vinos blancos secos, dulces y también vinos de postre.Pinot Grigio es una variedad de uva blanca que produce vinos blancos ligeros y refrescantes, con notas cítricas y florales.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
+  </si>
+  <si>
+    <t>Zinfandel</t>
+  </si>
+  <si>
+    <t>ZinfandelZinfandel</t>
+  </si>
+  <si>
+    <t>Cabernet</t>
+  </si>
+  <si>
+    <t>Bodega Seis</t>
+  </si>
+  <si>
+    <t>CabernetMerlot es una variedad de uva tinta que se caracteriza por su suavidad y sabor frutal en los vinos.Pinot Noir es una variedad de uva tinta que se asocia con vinos ligeros, elegantes y afrutados.</t>
+  </si>
+  <si>
+    <t>Pinot Noir</t>
+  </si>
+  <si>
+    <t>Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.Tannat es una variedad de uva tinta que se asocia principalmente con los vinos de Uruguay, conocidos por su estructura tánica y sabor intenso.</t>
+  </si>
+  <si>
+    <t>Torrontés</t>
+  </si>
+  <si>
+    <t>TorrontésRiesling es una variedad de uva blanca que puede producir desde vinos secos y refrescantes hasta vinos dulces y aromáticos.</t>
   </si>
 </sst>
 </file>
@@ -378,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -389,7 +446,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1150</v>
+        <v>1300</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -404,7 +461,7 @@
         <v>4</v>
       </c>
       <c r="G1">
-        <v>9</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -412,36 +469,36 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
       <c r="G2">
-        <v>7.9</v>
+        <v>9.199999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3">
-        <v>1200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -450,7 +507,168 @@
         <v>10</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1250</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>1350</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>1350</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>1100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>8.324999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>1300</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>8.300000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>1500</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>1150</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10">
+        <v>8.199999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Apply expert pattern in GestorRankingVinos.py
</commit_message>
<xml_diff>
--- a/RankingVinos.xlsx
+++ b/RankingVinos.xlsx
@@ -14,96 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
-  <si>
-    <t>Cabernet Franc</t>
-  </si>
-  <si>
-    <t>Bodega Cinco</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+  <si>
+    <t>Torrontés Clásico</t>
+  </si>
+  <si>
+    <t>Bodega Dos</t>
+  </si>
+  <si>
+    <t>Reconocida por sus Malbecs</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Torrontés ClásicoMourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
+  </si>
+  <si>
+    <t>Cabernet Sauvignon</t>
+  </si>
+  <si>
+    <t>Bodega Uno</t>
   </si>
   <si>
     <t>Famoso por sus vinos tintos de alta calidad</t>
   </si>
   <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Cabernet FrancSauvignon Blanc es una variedad de uva blanca conocida por su frescura y sus aromas herbáceos y cítricos.Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Sangiovese es una variedad de uva tinta que se asocia principalmente con los vinos italianos, conocidos por su acidez y sabor a frutas rojas.</t>
-  </si>
-  <si>
-    <t>Malbec</t>
-  </si>
-  <si>
-    <t>MalbecMalbec</t>
-  </si>
-  <si>
-    <t>Torrontés Clásico</t>
-  </si>
-  <si>
-    <t>Bodega Dos</t>
-  </si>
-  <si>
-    <t>Reconocida por sus Malbecs</t>
-  </si>
-  <si>
-    <t>Torrontés ClásicoMourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
-  </si>
-  <si>
-    <t>Merlot Reserva</t>
-  </si>
-  <si>
-    <t>Bodega Tres</t>
-  </si>
-  <si>
-    <t>Región importante de San Juan</t>
-  </si>
-  <si>
-    <t>Merlot ReservaMerlot Reserva</t>
-  </si>
-  <si>
-    <t>Riesling</t>
-  </si>
-  <si>
-    <t>Bodega Ocho</t>
-  </si>
-  <si>
-    <t>RieslingRiesling</t>
-  </si>
-  <si>
-    <t>Chardonnay</t>
-  </si>
-  <si>
-    <t>Bodega Cuatro</t>
-  </si>
-  <si>
-    <t>Sémillon es una variedad de uva blanca que se utiliza en la producción de vinos blancos secos, dulces y también vinos de postre.Pinot Grigio es una variedad de uva blanca que produce vinos blancos ligeros y refrescantes, con notas cítricas y florales.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
-  </si>
-  <si>
-    <t>Zinfandel</t>
-  </si>
-  <si>
-    <t>ZinfandelZinfandel</t>
-  </si>
-  <si>
-    <t>Cabernet</t>
-  </si>
-  <si>
-    <t>Bodega Seis</t>
-  </si>
-  <si>
-    <t>CabernetMerlot es una variedad de uva tinta que se caracteriza por su suavidad y sabor frutal en los vinos.Pinot Noir es una variedad de uva tinta que se asocia con vinos ligeros, elegantes y afrutados.</t>
-  </si>
-  <si>
-    <t>Pinot Noir</t>
-  </si>
-  <si>
-    <t>Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.Tannat es una variedad de uva tinta que se asocia principalmente con los vinos de Uruguay, conocidos por su estructura tánica y sabor intenso.</t>
-  </si>
-  <si>
-    <t>Torrontés</t>
-  </si>
-  <si>
-    <t>TorrontésRiesling es una variedad de uva blanca que puede producir desde vinos secos y refrescantes hasta vinos dulces y aromáticos.</t>
+    <t>Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.</t>
+  </si>
+  <si>
+    <t>Malbec Reserva</t>
+  </si>
+  <si>
+    <t>Mourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Grenache es una variedad de uva tinta que se utiliza en muchos vinos tintos y rosados, conocidos por su cuerpo y sabor afrutado.</t>
   </si>
 </sst>
 </file>
@@ -435,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -446,7 +389,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1300</v>
+        <v>1150</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -461,7 +404,7 @@
         <v>4</v>
       </c>
       <c r="G1">
-        <v>9.9</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -469,36 +412,36 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G2">
-        <v>9.199999999999999</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>1200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3">
-        <v>1150</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -507,168 +450,7 @@
         <v>10</v>
       </c>
       <c r="G3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>1250</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>1350</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>1350</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>1100</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7">
-        <v>8.324999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
-        <v>1300</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8">
-        <v>8.300000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9">
-        <v>1500</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9">
-        <v>8.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10">
-        <v>1150</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10">
-        <v>8.199999999999999</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Update database connection handling in database.py
</commit_message>
<xml_diff>
--- a/RankingVinos.xlsx
+++ b/RankingVinos.xlsx
@@ -14,7 +14,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+  <si>
+    <t>Cabernet Franc</t>
+  </si>
+  <si>
+    <t>Bodega Cinco</t>
+  </si>
+  <si>
+    <t>Famoso por sus vinos tintos de alta calidad</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Cabernet FrancSauvignon Blanc es una variedad de uva blanca conocida por su frescura y sus aromas herbáceos y cítricos.Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Sangiovese es una variedad de uva tinta que se asocia principalmente con los vinos italianos, conocidos por su acidez y sabor a frutas rojas.</t>
+  </si>
+  <si>
+    <t>Malbec</t>
+  </si>
+  <si>
+    <t>MalbecMalbec</t>
+  </si>
   <si>
     <t>Torrontés Clásico</t>
   </si>
@@ -25,28 +46,64 @@
     <t>Reconocida por sus Malbecs</t>
   </si>
   <si>
-    <t>Argentina</t>
-  </si>
-  <si>
     <t>Torrontés ClásicoMourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
   </si>
   <si>
-    <t>Cabernet Sauvignon</t>
-  </si>
-  <si>
-    <t>Bodega Uno</t>
-  </si>
-  <si>
-    <t>Famoso por sus vinos tintos de alta calidad</t>
-  </si>
-  <si>
-    <t>Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.</t>
-  </si>
-  <si>
-    <t>Malbec Reserva</t>
-  </si>
-  <si>
-    <t>Mourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Grenache es una variedad de uva tinta que se utiliza en muchos vinos tintos y rosados, conocidos por su cuerpo y sabor afrutado.</t>
+    <t>Merlot Reserva</t>
+  </si>
+  <si>
+    <t>Bodega Tres</t>
+  </si>
+  <si>
+    <t>Región importante de San Juan</t>
+  </si>
+  <si>
+    <t>Merlot ReservaMerlot Reserva</t>
+  </si>
+  <si>
+    <t>Riesling</t>
+  </si>
+  <si>
+    <t>Bodega Ocho</t>
+  </si>
+  <si>
+    <t>RieslingRiesling</t>
+  </si>
+  <si>
+    <t>Chardonnay</t>
+  </si>
+  <si>
+    <t>Bodega Cuatro</t>
+  </si>
+  <si>
+    <t>Sémillon es una variedad de uva blanca que se utiliza en la producción de vinos blancos secos, dulces y también vinos de postre.Pinot Grigio es una variedad de uva blanca que produce vinos blancos ligeros y refrescantes, con notas cítricas y florales.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
+  </si>
+  <si>
+    <t>Zinfandel</t>
+  </si>
+  <si>
+    <t>ZinfandelZinfandel</t>
+  </si>
+  <si>
+    <t>Cabernet</t>
+  </si>
+  <si>
+    <t>Bodega Seis</t>
+  </si>
+  <si>
+    <t>CabernetMerlot es una variedad de uva tinta que se caracteriza por su suavidad y sabor frutal en los vinos.Pinot Noir es una variedad de uva tinta que se asocia con vinos ligeros, elegantes y afrutados.</t>
+  </si>
+  <si>
+    <t>Pinot Noir</t>
+  </si>
+  <si>
+    <t>Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.Tannat es una variedad de uva tinta que se asocia principalmente con los vinos de Uruguay, conocidos por su estructura tánica y sabor intenso.</t>
+  </si>
+  <si>
+    <t>Torrontés</t>
+  </si>
+  <si>
+    <t>TorrontésRiesling es una variedad de uva blanca que puede producir desde vinos secos y refrescantes hasta vinos dulces y aromáticos.</t>
   </si>
 </sst>
 </file>
@@ -378,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -389,7 +446,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1150</v>
+        <v>1300</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -404,7 +461,7 @@
         <v>4</v>
       </c>
       <c r="G1">
-        <v>9</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -412,36 +469,36 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
       <c r="G2">
-        <v>7.9</v>
+        <v>9.199999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3">
-        <v>1200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -450,7 +507,168 @@
         <v>10</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1250</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>1350</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>1350</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>1100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>8.324999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>1300</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>8.300000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>1500</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>1150</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10">
+        <v>8.199999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
La vase de datos ahora esta en la nube
</commit_message>
<xml_diff>
--- a/RankingVinos.xlsx
+++ b/RankingVinos.xlsx
@@ -14,96 +14,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
-  <si>
-    <t>Cabernet Franc</t>
-  </si>
-  <si>
-    <t>Bodega Cinco</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+  <si>
+    <t>Torrontés Clásico</t>
+  </si>
+  <si>
+    <t>Bodega Dos</t>
+  </si>
+  <si>
+    <t>Reconocida por sus Malbecs</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Torrontés ClásicoMourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
+  </si>
+  <si>
+    <t>Merlot Reserva</t>
+  </si>
+  <si>
+    <t>Bodega Tres</t>
+  </si>
+  <si>
+    <t>Región importante de San Juan</t>
+  </si>
+  <si>
+    <t>Merlot ReservaMerlot Reserva</t>
+  </si>
+  <si>
+    <t>Chardonnay</t>
+  </si>
+  <si>
+    <t>Bodega Cuatro</t>
   </si>
   <si>
     <t>Famoso por sus vinos tintos de alta calidad</t>
   </si>
   <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Cabernet FrancSauvignon Blanc es una variedad de uva blanca conocida por su frescura y sus aromas herbáceos y cítricos.Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Sangiovese es una variedad de uva tinta que se asocia principalmente con los vinos italianos, conocidos por su acidez y sabor a frutas rojas.</t>
-  </si>
-  <si>
-    <t>Malbec</t>
-  </si>
-  <si>
-    <t>MalbecMalbec</t>
-  </si>
-  <si>
-    <t>Torrontés Clásico</t>
-  </si>
-  <si>
-    <t>Bodega Dos</t>
-  </si>
-  <si>
-    <t>Reconocida por sus Malbecs</t>
-  </si>
-  <si>
-    <t>Torrontés ClásicoMourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
-  </si>
-  <si>
-    <t>Merlot Reserva</t>
-  </si>
-  <si>
-    <t>Bodega Tres</t>
-  </si>
-  <si>
-    <t>Región importante de San Juan</t>
-  </si>
-  <si>
-    <t>Merlot ReservaMerlot Reserva</t>
-  </si>
-  <si>
-    <t>Riesling</t>
-  </si>
-  <si>
-    <t>Bodega Ocho</t>
-  </si>
-  <si>
-    <t>RieslingRiesling</t>
-  </si>
-  <si>
-    <t>Chardonnay</t>
-  </si>
-  <si>
-    <t>Bodega Cuatro</t>
-  </si>
-  <si>
     <t>Sémillon es una variedad de uva blanca que se utiliza en la producción de vinos blancos secos, dulces y también vinos de postre.Pinot Grigio es una variedad de uva blanca que produce vinos blancos ligeros y refrescantes, con notas cítricas y florales.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
   </si>
   <si>
-    <t>Zinfandel</t>
-  </si>
-  <si>
-    <t>ZinfandelZinfandel</t>
-  </si>
-  <si>
-    <t>Cabernet</t>
-  </si>
-  <si>
-    <t>Bodega Seis</t>
-  </si>
-  <si>
-    <t>CabernetMerlot es una variedad de uva tinta que se caracteriza por su suavidad y sabor frutal en los vinos.Pinot Noir es una variedad de uva tinta que se asocia con vinos ligeros, elegantes y afrutados.</t>
-  </si>
-  <si>
     <t>Pinot Noir</t>
   </si>
   <si>
     <t>Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.Tannat es una variedad de uva tinta que se asocia principalmente con los vinos de Uruguay, conocidos por su estructura tánica y sabor intenso.</t>
   </si>
   <si>
-    <t>Torrontés</t>
-  </si>
-  <si>
-    <t>TorrontésRiesling es una variedad de uva blanca que puede producir desde vinos secos y refrescantes hasta vinos dulces y aromáticos.</t>
+    <t>Cabernet Sauvignon</t>
+  </si>
+  <si>
+    <t>Bodega Uno</t>
+  </si>
+  <si>
+    <t>Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.</t>
+  </si>
+  <si>
+    <t>Malbec Reserva</t>
+  </si>
+  <si>
+    <t>Mourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Grenache es una variedad de uva tinta que se utiliza en muchos vinos tintos y rosados, conocidos por su cuerpo y sabor afrutado.</t>
   </si>
 </sst>
 </file>
@@ -435,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -446,7 +416,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1300</v>
+        <v>1150</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -461,7 +431,7 @@
         <v>4</v>
       </c>
       <c r="G1">
-        <v>9.9</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -469,59 +439,59 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1200</v>
+        <v>1250</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G2">
-        <v>9.199999999999999</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>1150</v>
+        <v>1350</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G3">
-        <v>9</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>1250</v>
+        <v>1500</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -530,7 +500,7 @@
         <v>14</v>
       </c>
       <c r="G4">
-        <v>8.9</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -538,13 +508,13 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>1350</v>
+        <v>1300</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -553,7 +523,7 @@
         <v>17</v>
       </c>
       <c r="G5">
-        <v>8.6</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -561,114 +531,22 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>1350</v>
+        <v>1200</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>1100</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7">
-        <v>8.324999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
-        <v>1300</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8">
-        <v>8.300000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9">
-        <v>1500</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9">
-        <v>8.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10">
-        <v>1150</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10">
-        <v>8.199999999999999</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Update Flask routes and templates for home and ranking pages
</commit_message>
<xml_diff>
--- a/RankingVinos.xlsx
+++ b/RankingVinos.xlsx
@@ -14,7 +14,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+  <si>
+    <t>Cabernet Franc</t>
+  </si>
+  <si>
+    <t>Bodega Cinco</t>
+  </si>
+  <si>
+    <t>Famoso por sus vinos tintos de alta calidad</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Cabernet FrancSauvignon Blanc es una variedad de uva blanca conocida por su frescura y sus aromas herbáceos y cítricos.Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Sangiovese es una variedad de uva tinta que se asocia principalmente con los vinos italianos, conocidos por su acidez y sabor a frutas rojas.</t>
+  </si>
+  <si>
+    <t>Malbec</t>
+  </si>
+  <si>
+    <t>MalbecMalbec</t>
+  </si>
   <si>
     <t>Torrontés Clásico</t>
   </si>
@@ -25,9 +46,6 @@
     <t>Reconocida por sus Malbecs</t>
   </si>
   <si>
-    <t>Argentina</t>
-  </si>
-  <si>
     <t>Torrontés ClásicoMourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
   </si>
   <si>
@@ -43,37 +61,49 @@
     <t>Merlot ReservaMerlot Reserva</t>
   </si>
   <si>
+    <t>Riesling</t>
+  </si>
+  <si>
+    <t>Bodega Ocho</t>
+  </si>
+  <si>
+    <t>RieslingRiesling</t>
+  </si>
+  <si>
     <t>Chardonnay</t>
   </si>
   <si>
     <t>Bodega Cuatro</t>
   </si>
   <si>
-    <t>Famoso por sus vinos tintos de alta calidad</t>
-  </si>
-  <si>
     <t>Sémillon es una variedad de uva blanca que se utiliza en la producción de vinos blancos secos, dulces y también vinos de postre.Pinot Grigio es una variedad de uva blanca que produce vinos blancos ligeros y refrescantes, con notas cítricas y florales.Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.</t>
   </si>
   <si>
+    <t>Zinfandel</t>
+  </si>
+  <si>
+    <t>ZinfandelZinfandel</t>
+  </si>
+  <si>
+    <t>Cabernet</t>
+  </si>
+  <si>
+    <t>Bodega Seis</t>
+  </si>
+  <si>
+    <t>CabernetMerlot es una variedad de uva tinta que se caracteriza por su suavidad y sabor frutal en los vinos.Pinot Noir es una variedad de uva tinta que se asocia con vinos ligeros, elegantes y afrutados.</t>
+  </si>
+  <si>
     <t>Pinot Noir</t>
   </si>
   <si>
     <t>Garnacha Blanca es una variedad de uva blanca que produce vinos blancos con cuerpo y textura, con sabores a frutas blancas y notas florales.Tannat es una variedad de uva tinta que se asocia principalmente con los vinos de Uruguay, conocidos por su estructura tánica y sabor intenso.</t>
   </si>
   <si>
-    <t>Cabernet Sauvignon</t>
-  </si>
-  <si>
-    <t>Bodega Uno</t>
-  </si>
-  <si>
-    <t>Bonarda es una variedad de uva tinta que se utiliza en la producción de vinos tintos suaves y afrutados, con sabores a frutas negras y especias.Cabernet Sauvignon es una variedad de uva tinta ampliamente reconocida por su presencia en los vinos tintos de Bordeaux.</t>
-  </si>
-  <si>
-    <t>Malbec Reserva</t>
-  </si>
-  <si>
-    <t>Mourvèdre es una variedad de uva tinta que se utiliza en la producción de vinos tintos robustos y especiados.Grenache es una variedad de uva tinta que se utiliza en muchos vinos tintos y rosados, conocidos por su cuerpo y sabor afrutado.</t>
+    <t>Torrontés</t>
+  </si>
+  <si>
+    <t>TorrontésRiesling es una variedad de uva blanca que puede producir desde vinos secos y refrescantes hasta vinos dulces y aromáticos.</t>
   </si>
 </sst>
 </file>
@@ -405,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -416,7 +446,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1150</v>
+        <v>1300</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -431,7 +461,7 @@
         <v>4</v>
       </c>
       <c r="G1">
-        <v>9</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -439,59 +469,59 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1250</v>
+        <v>1200</v>
       </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
       <c r="G2">
-        <v>8.9</v>
+        <v>9.199999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>1350</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
       <c r="G3">
-        <v>8.4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1250</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4">
-        <v>1500</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -500,7 +530,7 @@
         <v>14</v>
       </c>
       <c r="G4">
-        <v>8.25</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -508,13 +538,13 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>1300</v>
+        <v>1350</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -523,7 +553,7 @@
         <v>17</v>
       </c>
       <c r="G5">
-        <v>7.9</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -531,22 +561,114 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>1200</v>
+        <v>1350</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>1100</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>8.324999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>1300</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>8.300000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>1500</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>1150</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10">
+        <v>8.199999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>